<commit_message>
Updated data in readme file.
</commit_message>
<xml_diff>
--- a/data/UseOfForceData.xlsx
+++ b/data/UseOfForceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\UseOfForce\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B1C0EB-863E-49F6-8B61-59DB0D02445E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F14109-136C-4CD8-AB10-A25FF94D9958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7200" windowWidth="29040" windowHeight="15225" activeTab="1" xr2:uid="{CD62EF23-FE4D-4401-B457-9850FA22DBB8}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{CD62EF23-FE4D-4401-B457-9850FA22DBB8}"/>
   </bookViews>
   <sheets>
     <sheet name="State Template" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Latitude of the event</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Geographic coordinate system</t>
+  </si>
+  <si>
+    <t>Use of force definition</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Use_of_force</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D9A545-40AE-44A0-9467-4BEA13873DB1}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -512,10 +518,19 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C6AB70AC-2282-461E-A1D6-CE4B977FD041}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{E68103A8-8287-43F3-AD62-D450AA4EC5B9}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{82573842-7F1F-489F-86C2-073270D77E1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>